<commit_message>
Refining core data set
</commit_message>
<xml_diff>
--- a/tabular/a3-side-data.xlsx
+++ b/tabular/a3-side-data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/host/A3G-GLUE/tabular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0EDD94-BECC-7B42-B5A6-F1F538B8ED08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5556B68-E0F1-104B-8C70-BB81F213BA12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="960" windowWidth="25000" windowHeight="12860" xr2:uid="{DEC304A4-634A-1447-93DC-41EE14289173}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="164">
   <si>
     <t>SequenceID</t>
   </si>
@@ -48,9 +49,6 @@
     <t>Species</t>
   </si>
   <si>
-    <t>Order</t>
-  </si>
-  <si>
     <t>NM_20661.2</t>
   </si>
   <si>
@@ -157,9 +155,6 @@
   </si>
   <si>
     <t>A3Z3</t>
-  </si>
-  <si>
-    <t>NP_084531.2</t>
   </si>
   <si>
     <t>APOBEC3</t>
@@ -499,6 +494,51 @@
   </si>
   <si>
     <t>XP_2186660.1</t>
+  </si>
+  <si>
+    <t>sequenceID</t>
+  </si>
+  <si>
+    <t>gene_id_old</t>
+  </si>
+  <si>
+    <t>gene_id</t>
+  </si>
+  <si>
+    <t>organism</t>
+  </si>
+  <si>
+    <t>organism_tax_order</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>confirmed_mRNA</t>
+  </si>
+  <si>
+    <t>predicted_mRNA</t>
+  </si>
+  <si>
+    <t>KX241572</t>
+  </si>
+  <si>
+    <t>NM_20661</t>
+  </si>
+  <si>
+    <t>NM_203454</t>
+  </si>
+  <si>
+    <t>NM_6789</t>
+  </si>
+  <si>
+    <t>NM_1644</t>
+  </si>
+  <si>
+    <t>NM_181773</t>
+  </si>
+  <si>
+    <t>full_name</t>
   </si>
 </sst>
 </file>
@@ -566,12 +606,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -886,384 +932,410 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC05A690-FA98-4941-B089-B2E5CA7953DF}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="E7" sqref="A1:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="15.1640625" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" customWidth="1"/>
+    <col min="6" max="6" width="25.83203125" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G2" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G3" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G4" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="G6" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="G7" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="G8" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="B9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="G9" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="B10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="G10" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="G11" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="D13" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>46</v>
+        <v>157</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>50</v>
+        <v>56</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>157</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>59</v>
+      <c r="G17" s="2" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -1275,7 +1347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA44EABB-9F5C-414E-8648-C99D70B1537A}">
   <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
@@ -1302,872 +1374,872 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="D9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D33" t="s">
         <v>95</v>
-      </c>
-      <c r="B33" t="s">
-        <v>96</v>
-      </c>
-      <c r="D33" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" t="s">
+        <v>97</v>
+      </c>
+      <c r="D34" t="s">
         <v>98</v>
-      </c>
-      <c r="B34" t="s">
-        <v>99</v>
-      </c>
-      <c r="D34" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D35" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D36" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B37" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B39" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" t="s">
         <v>36</v>
-      </c>
-      <c r="B40" t="s">
-        <v>20</v>
-      </c>
-      <c r="D40" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D42" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B43" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D43" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D44" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B45" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D45" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D46" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B47" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D47" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B48" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D48" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B49" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D49" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B50" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D50" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B51" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D51" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B52" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D52" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B53" t="s">
+        <v>40</v>
+      </c>
+      <c r="D53" t="s">
         <v>42</v>
-      </c>
-      <c r="D53" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B54" t="s">
+        <v>40</v>
+      </c>
+      <c r="D54" t="s">
         <v>42</v>
-      </c>
-      <c r="D54" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B55" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D55" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B56" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D56" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B57" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D57" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B58" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D58" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B59" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D59" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B60" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D60" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B61" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D61" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B62" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D62" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B63" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D63" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B64" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D64" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>54</v>
+      </c>
+      <c r="B65" t="s">
+        <v>55</v>
+      </c>
+      <c r="D65" t="s">
         <v>56</v>
-      </c>
-      <c r="B65" t="s">
-        <v>57</v>
-      </c>
-      <c r="D65" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B66" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D66" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B67" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D67" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B68" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D68" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B69" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D69" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B70" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D70" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B71" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D71" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B72" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D72" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B73" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D73" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B74" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D74" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B75" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D75" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B76" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D76" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2177,4 +2249,89 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E297C109-A83D-364E-BF19-31FF296D3873}">
+  <dimension ref="B1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated tabular data (standardising nomenclature)
</commit_message>
<xml_diff>
--- a/tabular/a3-side-data.xlsx
+++ b/tabular/a3-side-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/host/A3G-GLUE/tabular/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/host/A3G-GLUE/tabular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA4DBE8-4751-E040-AD53-4AF903E17D29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC2A8EF-4933-4446-B35C-BF86D3060A0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="960" windowWidth="25000" windowHeight="12860" xr2:uid="{DEC304A4-634A-1447-93DC-41EE14289173}"/>
+    <workbookView xWindow="14780" yWindow="4460" windowWidth="25000" windowHeight="12860" xr2:uid="{DEC304A4-634A-1447-93DC-41EE14289173}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="181">
   <si>
     <t>SequenceID</t>
   </si>
@@ -115,25 +115,16 @@
     <t>APOBEC3Fv1</t>
   </si>
   <si>
-    <t>A3F</t>
-  </si>
-  <si>
     <t>NM_021822</t>
   </si>
   <si>
     <t>APOBEC3G</t>
   </si>
   <si>
-    <t>A3G</t>
-  </si>
-  <si>
     <t>NM_181773.4</t>
   </si>
   <si>
     <t>APOBEC3H</t>
-  </si>
-  <si>
-    <t>A3H</t>
   </si>
   <si>
     <t>NM_203454.2</t>
@@ -523,22 +514,82 @@
     <t>KX241572</t>
   </si>
   <si>
-    <t>NM_20661</t>
-  </si>
-  <si>
     <t>NM_203454</t>
   </si>
   <si>
-    <t>NM_6789</t>
-  </si>
-  <si>
-    <t>NM_1644</t>
-  </si>
-  <si>
     <t>NM_181773</t>
   </si>
   <si>
     <t>full_name</t>
+  </si>
+  <si>
+    <t>A3Z1a</t>
+  </si>
+  <si>
+    <t>A3Z2a-A3Z1b</t>
+  </si>
+  <si>
+    <t>A3Z2b</t>
+  </si>
+  <si>
+    <t>A3Z2c-A3Z2d</t>
+  </si>
+  <si>
+    <t>A3Z2e-A3Z2f</t>
+  </si>
+  <si>
+    <t>A3Z2g-A3Z1c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homo sapiens apolipoprotein B mRNA editing enzyme catalytic subunit 3B </t>
+  </si>
+  <si>
+    <t>Homo sapiens apolipoprotein B mRNA editing enzyme catalytic subunit 3C</t>
+  </si>
+  <si>
+    <t>Homo sapiens apolipoprotein B mRNA editing enzyme catalytic subunit 3D</t>
+  </si>
+  <si>
+    <t>Homo sapiens apolipoprotein B mRNA editing enzyme catalytic subunit 3F</t>
+  </si>
+  <si>
+    <t>Homo sapiens apolipoprotein B mRNA editing enzyme catalytic subunit 3G</t>
+  </si>
+  <si>
+    <t>Homo sapiens apolipoprotein B mRNA editing enzyme catalytic subunit 3H</t>
+  </si>
+  <si>
+    <t>Homo sapiens apolipoprotein B mRNA editing enzyme catalytic polypeptide like 4</t>
+  </si>
+  <si>
+    <t>Homo sapiens apolipoprotein B mRNA editing enzyme catalytic subunit 3A</t>
+  </si>
+  <si>
+    <t>NM_020661</t>
+  </si>
+  <si>
+    <t>Homo sapiens activation induced cytidine deaminase</t>
+  </si>
+  <si>
+    <t>NM_000384</t>
+  </si>
+  <si>
+    <t>NM_001644</t>
+  </si>
+  <si>
+    <t>Homo sapiens apolipoprotein B mRNA editing enzyme catalytic subunit 2</t>
+  </si>
+  <si>
+    <t>Homo sapiens apolipoprotein B mRNA editing enzyme catalytic subunit 1</t>
+  </si>
+  <si>
+    <t>Bos taurus apolipoprotein B mRNA</t>
+  </si>
+  <si>
+    <t>Pteropus vampyrus apolipoprotein B mRNA editing enzyme, catalytic polypeptide-like 3</t>
+  </si>
+  <si>
+    <t>Equus caballus apolipoprotein B mRNA editing enzyme catalytic subunit 3H</t>
   </si>
 </sst>
 </file>
@@ -935,13 +986,15 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="A1:G17"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="15.1640625" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="83.33203125" customWidth="1"/>
     <col min="5" max="5" width="23.6640625" customWidth="1"/>
     <col min="6" max="6" width="25.83203125" customWidth="1"/>
     <col min="7" max="7" width="20.83203125" customWidth="1"/>
@@ -949,30 +1002,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>151</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -981,7 +1034,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>173</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>6</v>
@@ -990,12 +1043,12 @@
         <v>7</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -1004,7 +1057,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
+        <v>177</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>6</v>
@@ -1013,12 +1066,12 @@
         <v>7</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>11</v>
@@ -1027,7 +1080,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>176</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>6</v>
@@ -1036,21 +1089,21 @@
         <v>7</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>158</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>14</v>
+        <v>171</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>6</v>
@@ -1059,7 +1112,7 @@
         <v>7</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1070,10 +1123,10 @@
         <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>159</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>17</v>
+        <v>164</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>6</v>
@@ -1082,7 +1135,7 @@
         <v>7</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1093,10 +1146,10 @@
         <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>20</v>
+        <v>160</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>20</v>
+        <v>165</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>6</v>
@@ -1105,7 +1158,7 @@
         <v>7</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1116,10 +1169,10 @@
         <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>23</v>
+        <v>161</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>23</v>
+        <v>166</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>6</v>
@@ -1128,7 +1181,7 @@
         <v>7</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1139,10 +1192,10 @@
         <v>25</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>26</v>
+        <v>162</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>26</v>
+        <v>167</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>6</v>
@@ -1151,21 +1204,21 @@
         <v>7</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="C10" s="2" t="s">
-        <v>29</v>
+        <v>163</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>29</v>
+        <v>168</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>6</v>
@@ -1174,21 +1227,21 @@
         <v>7</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>32</v>
+        <v>169</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>6</v>
@@ -1197,21 +1250,21 @@
         <v>7</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>34</v>
+        <v>170</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>6</v>
@@ -1220,122 +1273,122 @@
         <v>7</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="4" t="s">
+      <c r="G14" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="C15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="F15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>57</v>
+      <c r="D16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>157</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>57</v>
+      <c r="A17" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -1430,10 +1483,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
@@ -1496,10 +1549,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
@@ -1508,10 +1561,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
@@ -1520,10 +1573,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
@@ -1532,10 +1585,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
@@ -1544,10 +1597,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
@@ -1556,22 +1609,22 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
@@ -1580,666 +1633,666 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B33" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D33" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B34" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D34" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D35" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D36" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B37" t="s">
         <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B38" t="s">
         <v>9</v>
       </c>
       <c r="D38" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B39" t="s">
         <v>11</v>
       </c>
       <c r="D39" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B40" t="s">
         <v>19</v>
       </c>
       <c r="D40" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D41" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B42" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D42" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B43" t="s">
         <v>5</v>
       </c>
       <c r="D43" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B44" t="s">
         <v>9</v>
       </c>
       <c r="D44" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B45" t="s">
         <v>11</v>
       </c>
       <c r="D45" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B46" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D46" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B47" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D47" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B48" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D48" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B49" t="s">
         <v>13</v>
       </c>
       <c r="D49" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B50" t="s">
         <v>5</v>
       </c>
       <c r="D50" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B51" t="s">
         <v>9</v>
       </c>
       <c r="D51" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B52" t="s">
         <v>11</v>
       </c>
       <c r="D52" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B53" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D53" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B54" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D54" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B55" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D55" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B56" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D56" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B57" t="s">
         <v>16</v>
       </c>
       <c r="D57" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B58" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D58" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B59" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D59" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B60" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D60" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B61" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D61" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B62" t="s">
         <v>5</v>
       </c>
       <c r="D62" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B63" t="s">
         <v>9</v>
       </c>
       <c r="D63" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B64" t="s">
         <v>11</v>
       </c>
       <c r="D64" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B65" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D65" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B66" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D66" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B67" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D67" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B68" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D68" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B69" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D69" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B70" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D70" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B71" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D71" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B72" t="s">
         <v>13</v>
       </c>
       <c r="D72" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B73" t="s">
         <v>16</v>
       </c>
       <c r="D73" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B74" t="s">
         <v>5</v>
       </c>
       <c r="D74" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B75" t="s">
         <v>9</v>
       </c>
       <c r="D75" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B76" t="s">
         <v>11</v>
       </c>
       <c r="D76" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2269,38 +2322,38 @@
         <v>19</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
@@ -2308,13 +2361,13 @@
         <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
@@ -2322,13 +2375,13 @@
         <v>16</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>